<commit_message>
liwc data and code
</commit_message>
<xml_diff>
--- a/data/1b.xlsx
+++ b/data/1b.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\2021 Fall\EDLD654 - Machine Learning\text-analysis-of-conflicts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E4457D-0B2D-457D-86A0-192DE3FA7C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075C494F-17E5-4D02-AC88-CB0E8681D3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2972" uniqueCount="1009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2971" uniqueCount="1008">
   <si>
     <t>age</t>
   </si>
@@ -3047,9 +3047,6 @@
   </si>
   <si>
     <t>non-binary</t>
-  </si>
-  <si>
-    <t>race_other</t>
   </si>
 </sst>
 </file>
@@ -3398,10 +3395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J993"/>
+  <dimension ref="A1:I993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3410,7 +3407,7 @@
     <col min="4" max="8" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1004</v>
       </c>
@@ -3438,11 +3435,8 @@
       <c r="I1" s="2" t="s">
         <v>1002</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>14</v>
       </c>
@@ -3468,7 +3462,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>19</v>
       </c>
@@ -3494,7 +3488,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>51</v>
       </c>
@@ -3520,7 +3514,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>52</v>
       </c>
@@ -3546,7 +3540,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>61</v>
       </c>
@@ -3572,7 +3566,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>65</v>
       </c>
@@ -3598,7 +3592,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>76</v>
       </c>
@@ -3624,7 +3618,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>78</v>
       </c>
@@ -3650,7 +3644,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>83</v>
       </c>
@@ -3676,7 +3670,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>94</v>
       </c>
@@ -3702,7 +3696,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>96</v>
       </c>
@@ -3728,7 +3722,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>101</v>
       </c>
@@ -3754,7 +3748,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>125</v>
       </c>
@@ -3780,7 +3774,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>132</v>
       </c>
@@ -3806,7 +3800,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>133</v>
       </c>
@@ -29175,6 +29169,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I993" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>